<commit_message>
Clock weigth calc + bugs + new special
</commit_message>
<xml_diff>
--- a/static/data/data.xlsx
+++ b/static/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\churc\Church\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\Church\Church\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0861D6B-60DA-4D3B-8BA0-E9EA762F9379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7914DED1-DD49-4D83-9E6C-F5B5E222FA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCEA294A-4ACF-4234-BA0E-D22A7860C650}"/>
+    <workbookView xWindow="3780" yWindow="3735" windowWidth="28800" windowHeight="15435" xr2:uid="{FCEA294A-4ACF-4234-BA0E-D22A7860C650}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="137">
   <si>
     <t>Typ</t>
   </si>
@@ -420,6 +420,39 @@
   </si>
   <si>
     <t>3C Kopparplåt</t>
+  </si>
+  <si>
+    <t>Takryttare</t>
+  </si>
+  <si>
+    <t>Pris 2019</t>
+  </si>
+  <si>
+    <t>Höjd 0-3 m</t>
+  </si>
+  <si>
+    <t>Höjd 3-6 m</t>
+  </si>
+  <si>
+    <t>Höjd &gt;6m</t>
+  </si>
+  <si>
+    <t>Fial</t>
+  </si>
+  <si>
+    <t>Höjd</t>
+  </si>
+  <si>
+    <t>Typ 1</t>
+  </si>
+  <si>
+    <t>0-3m</t>
+  </si>
+  <si>
+    <t>Typ 2</t>
+  </si>
+  <si>
+    <t>&gt;3m</t>
   </si>
 </sst>
 </file>
@@ -509,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -527,6 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,7 +914,7 @@
     <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.140625" customWidth="1"/>
+    <col min="39" max="39" width="12" customWidth="1"/>
     <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -996,6 +1030,18 @@
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
+      <c r="AL3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1108,6 +1154,30 @@
       </c>
       <c r="AK4" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.25">
@@ -1227,6 +1297,32 @@
       <c r="AK5" s="16">
         <f t="shared" si="5"/>
         <v>3873.9375</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN5">
+        <v>6500</v>
+      </c>
+      <c r="AO5" s="17">
+        <f>AN5*Prishöjningsfaktor_FPI*Moms</f>
+        <v>111913.75</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR5">
+        <v>6500</v>
+      </c>
+      <c r="AS5" s="17">
+        <f>AR5*Prishöjningsfaktor_FPI*Moms</f>
+        <v>111913.75</v>
       </c>
       <c r="BF5" s="6"/>
       <c r="BG5" s="6"/>
@@ -1348,6 +1444,32 @@
         <f t="shared" si="5"/>
         <v>4132.2000000000007</v>
       </c>
+      <c r="AL6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN6">
+        <v>13000</v>
+      </c>
+      <c r="AO6" s="17">
+        <f>AN6*Prishöjningsfaktor_FPI*Moms</f>
+        <v>223827.5</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR6">
+        <v>13000</v>
+      </c>
+      <c r="AS6" s="17">
+        <f>AR6*Prishöjningsfaktor_FPI*Moms</f>
+        <v>223827.5</v>
+      </c>
       <c r="BP6" s="6"/>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.25">
@@ -1367,7 +1489,7 @@
         <v>250</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" ref="I5:I30" si="6">1.1+(G7/jmfpris_vagg)/100</f>
+        <f t="shared" ref="I7:I30" si="6">1.1+(G7/jmfpris_vagg)/100</f>
         <v>1.1564864864864866</v>
       </c>
       <c r="J7" s="7" t="s">
@@ -1459,6 +1581,19 @@
         <f t="shared" si="5"/>
         <v>3873.9375</v>
       </c>
+      <c r="AL7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN7">
+        <v>33000</v>
+      </c>
+      <c r="AO7" s="17">
+        <f>AN7*Prishöjningsfaktor_FPI*Moms</f>
+        <v>568177.50000000012</v>
+      </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="D8" s="7" t="s">
@@ -2461,7 +2596,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB19" xr:uid="{81FA3817-5029-4E85-B009-42D1A0154D3B}">
       <formula1>$Z$18:$Z$21</formula1>
     </dataValidation>
@@ -2472,12 +2607,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100E3A94D389FFE264EB2F3F6B1F57230B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="35eb813f27fef671c6204ac456ba59d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="42f6929c-7497-4fbc-999b-8d8ce8f715aa" xmlns:ns3="dc085be0-fca3-4993-9674-220bf0b75bb4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eaf7d27e9017643da0db6c02cd482c23" ns2:_="" ns3:_="">
     <xsd:import namespace="42f6929c-7497-4fbc-999b-8d8ce8f715aa"/>
@@ -2694,16 +2838,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5760F594-140A-4149-87CB-281F2DB2C0D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C17887C4-F280-4802-97C9-20237DE9C8EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2712,7 +2855,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF63EF48-BFE5-481B-986C-BEDE8FE8D22D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2729,12 +2872,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5760F594-140A-4149-87CB-281F2DB2C0D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
images + new facts + better sum
</commit_message>
<xml_diff>
--- a/static/data/data.xlsx
+++ b/static/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\Church\Church\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7914DED1-DD49-4D83-9E6C-F5B5E222FA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EF242-657C-45B6-B5A4-484EE284BCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3735" windowWidth="28800" windowHeight="15435" xr2:uid="{FCEA294A-4ACF-4234-BA0E-D22A7860C650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FCEA294A-4ACF-4234-BA0E-D22A7860C650}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -555,7 +555,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -875,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA15BB0-045F-452E-94B0-E87CF353FA42}">
-  <dimension ref="A1:BP31"/>
+  <dimension ref="A1:BP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +913,7 @@
     <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12" customWidth="1"/>
+    <col min="39" max="39" width="6.140625" customWidth="1"/>
     <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -943,15 +942,15 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <f>MIN(G5:G30)</f>
         <v>185</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="14">
         <f>MIN(L5:L10)</f>
         <v>140</v>
       </c>
-      <c r="P2" s="15">
+      <c r="P2" s="14">
         <f t="shared" ref="P2:R2" si="0">MIN(P5:P10)</f>
         <v>160</v>
       </c>
@@ -963,7 +962,7 @@
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="X2" s="15">
+      <c r="X2" s="14">
         <f>MIN(X5:X15)</f>
         <v>100</v>
       </c>
@@ -1184,11 +1183,11 @@
       <c r="A5">
         <v>1377.4</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <f>A5/100</f>
         <v>13.774000000000001</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>1.25</v>
       </c>
       <c r="D5" t="s">
@@ -1207,8 +1206,8 @@
         <v>250</v>
       </c>
       <c r="I5" s="10">
-        <f>1.1+(G5/jmfpris_vagg)/100</f>
-        <v>1.1470270270270271</v>
+        <f xml:space="preserve"> 0.0010062893081761*G5+ 0.748427672955975</f>
+        <v>1.6238993710691818</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
@@ -1216,12 +1215,12 @@
       <c r="K5" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>140</v>
       </c>
       <c r="M5" s="10">
-        <f t="shared" ref="M5:M10" si="1">1.1+(L5/140)/100</f>
-        <v>1.1100000000000001</v>
+        <f>0.00432432432432432*L5 + 0.394594594594595</f>
+        <v>0.99999999999999978</v>
       </c>
       <c r="N5" t="s">
         <v>13</v>
@@ -1237,12 +1236,12 @@
       </c>
       <c r="S5" s="8"/>
       <c r="T5" s="10">
-        <f t="shared" ref="T5:U10" si="2">1.1+(Q5/jmfpris_innertak)/100</f>
-        <v>1.1353125000000002</v>
+        <f xml:space="preserve"> 0.00253968253968254*Q5 + 0.365079365079365</f>
+        <v>1.8000000000000003</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1515625</v>
+        <f xml:space="preserve"> 0.0016*R5 + 0.48</f>
+        <v>1.8</v>
       </c>
       <c r="V5" t="s">
         <v>13</v>
@@ -1250,19 +1249,19 @@
       <c r="W5" t="s">
         <v>105</v>
       </c>
-      <c r="X5" s="13">
+      <c r="X5" s="12">
         <v>100</v>
       </c>
       <c r="Y5">
         <v>150</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" ref="Z5:Z13" si="3">1.1+(X5/jmfpris_yttertak)/100</f>
-        <v>1.1100000000000001</v>
+        <f xml:space="preserve"> 0.00355555555555556*X5 + 0.644444444444444</f>
+        <v>1</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ref="AA5:AA13" si="4">1.1+(Y5/jmfpris_yttertak)/100</f>
-        <v>1.115</v>
+        <f xml:space="preserve"> 0.00238805970149254*Y5 + 0.641791044776119</f>
+        <v>1</v>
       </c>
       <c r="AB5" t="s">
         <v>13</v>
@@ -1282,20 +1281,20 @@
       <c r="AG5">
         <v>225</v>
       </c>
-      <c r="AH5" s="16">
+      <c r="AH5" s="15">
         <f>AD5*Prishöjningsfaktor_FPI*Moms</f>
         <v>2324.3625000000002</v>
       </c>
-      <c r="AI5" s="16">
-        <f t="shared" ref="AH5:AK14" si="5">AE5*Prishöjningsfaktor_FPI*Moms</f>
+      <c r="AI5" s="15">
+        <f t="shared" ref="AH5:AK14" si="1">AE5*Prishöjningsfaktor_FPI*Moms</f>
         <v>2410.4500000000003</v>
       </c>
-      <c r="AJ5" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ5" s="15">
+        <f t="shared" si="1"/>
         <v>3099.15</v>
       </c>
-      <c r="AK5" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK5" s="15">
+        <f t="shared" si="1"/>
         <v>3873.9375</v>
       </c>
       <c r="AL5" t="s">
@@ -1307,7 +1306,7 @@
       <c r="AN5">
         <v>6500</v>
       </c>
-      <c r="AO5" s="17">
+      <c r="AO5" s="16">
         <f>AN5*Prishöjningsfaktor_FPI*Moms</f>
         <v>111913.75</v>
       </c>
@@ -1320,7 +1319,7 @@
       <c r="AR5">
         <v>6500</v>
       </c>
-      <c r="AS5" s="17">
+      <c r="AS5" s="16">
         <f>AR5*Prishöjningsfaktor_FPI*Moms</f>
         <v>111913.75</v>
       </c>
@@ -1352,8 +1351,8 @@
         <v>250</v>
       </c>
       <c r="I6" s="10">
-        <f>1.1+(G6/jmfpris_vagg)/100</f>
-        <v>1.1516216216216217</v>
+        <f t="shared" ref="I6:I30" si="2" xml:space="preserve"> 0.0010062893081761*G6+ 0.748427672955975</f>
+        <v>1.7094339622641503</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
@@ -1365,8 +1364,8 @@
         <v>255</v>
       </c>
       <c r="M6" s="10">
-        <f t="shared" si="1"/>
-        <v>1.1182142857142858</v>
+        <f t="shared" ref="M6:M10" si="3">0.00432432432432432*L6 + 0.394594594594595</f>
+        <v>1.4972972972972967</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>15</v>
@@ -1383,12 +1382,12 @@
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1271875</v>
+        <f t="shared" ref="T6:T10" si="4" xml:space="preserve"> 0.00253968253968254*Q6 + 0.365079365079365</f>
+        <v>1.4698412698412699</v>
       </c>
       <c r="U6" s="10">
-        <f>1.1+(R6/jmfpris_innertak)/100</f>
-        <v>1.1409375000000002</v>
+        <f t="shared" ref="U6:U10" si="5" xml:space="preserve"> 0.0016*R6 + 0.48</f>
+        <v>1.528</v>
       </c>
       <c r="V6" t="s">
         <v>14</v>
@@ -1403,12 +1402,12 @@
         <v>180</v>
       </c>
       <c r="Z6" s="10">
-        <f t="shared" si="3"/>
-        <v>1.1120000000000001</v>
+        <f t="shared" ref="Z6:Z15" si="6" xml:space="preserve"> 0.00355555555555556*X6 + 0.644444444444444</f>
+        <v>1.0711111111111111</v>
       </c>
       <c r="AA6" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1180000000000001</v>
+        <f t="shared" ref="AA6:AA15" si="7" xml:space="preserve"> 0.00238805970149254*Y6 + 0.641791044776119</f>
+        <v>1.0716417910447762</v>
       </c>
       <c r="AB6" t="s">
         <v>14</v>
@@ -1428,20 +1427,20 @@
       <c r="AG6">
         <v>240</v>
       </c>
-      <c r="AH6" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH6" s="15">
+        <f t="shared" si="1"/>
         <v>2582.6250000000005</v>
       </c>
-      <c r="AI6" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI6" s="15">
+        <f t="shared" si="1"/>
         <v>2840.8874999999998</v>
       </c>
-      <c r="AJ6" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ6" s="15">
+        <f t="shared" si="1"/>
         <v>3271.3250000000007</v>
       </c>
-      <c r="AK6" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK6" s="15">
+        <f t="shared" si="1"/>
         <v>4132.2000000000007</v>
       </c>
       <c r="AL6" t="s">
@@ -1453,7 +1452,7 @@
       <c r="AN6">
         <v>13000</v>
       </c>
-      <c r="AO6" s="17">
+      <c r="AO6" s="16">
         <f>AN6*Prishöjningsfaktor_FPI*Moms</f>
         <v>223827.5</v>
       </c>
@@ -1466,7 +1465,7 @@
       <c r="AR6">
         <v>13000</v>
       </c>
-      <c r="AS6" s="17">
+      <c r="AS6" s="16">
         <f>AR6*Prishöjningsfaktor_FPI*Moms</f>
         <v>223827.5</v>
       </c>
@@ -1489,8 +1488,8 @@
         <v>250</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" ref="I7:I30" si="6">1.1+(G7/jmfpris_vagg)/100</f>
-        <v>1.1564864864864866</v>
+        <f t="shared" si="2"/>
+        <v>1.7999999999999994</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
@@ -1501,9 +1500,9 @@
       <c r="L7" s="7">
         <v>220</v>
       </c>
-      <c r="M7" s="12">
-        <f t="shared" si="1"/>
-        <v>1.1157142857142859</v>
+      <c r="M7" s="10">
+        <f t="shared" si="3"/>
+        <v>1.3459459459459455</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>16</v>
@@ -1520,12 +1519,12 @@
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
+        <f t="shared" si="4"/>
+        <v>1.5841269841269843</v>
       </c>
       <c r="U7" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1434375000000001</v>
+        <f t="shared" si="5"/>
+        <v>1.5920000000000001</v>
       </c>
       <c r="V7" t="s">
         <v>46</v>
@@ -1540,12 +1539,12 @@
         <v>255</v>
       </c>
       <c r="Z7" s="10">
-        <f t="shared" si="3"/>
-        <v>1.117</v>
+        <f t="shared" si="6"/>
+        <v>1.2488888888888892</v>
       </c>
       <c r="AA7" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1255000000000002</v>
+        <f t="shared" si="7"/>
+        <v>1.2507462686567168</v>
       </c>
       <c r="AB7" t="s">
         <v>46</v>
@@ -1565,20 +1564,20 @@
       <c r="AG7">
         <v>225</v>
       </c>
-      <c r="AH7" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH7" s="15">
+        <f t="shared" si="1"/>
         <v>2324.3625000000002</v>
       </c>
-      <c r="AI7" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI7" s="15">
+        <f t="shared" si="1"/>
         <v>2410.4500000000003</v>
       </c>
-      <c r="AJ7" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ7" s="15">
+        <f t="shared" si="1"/>
         <v>3099.15</v>
       </c>
-      <c r="AK7" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK7" s="15">
+        <f t="shared" si="1"/>
         <v>3873.9375</v>
       </c>
       <c r="AL7" t="s">
@@ -1590,7 +1589,7 @@
       <c r="AN7">
         <v>33000</v>
       </c>
-      <c r="AO7" s="17">
+      <c r="AO7" s="16">
         <f>AN7*Prishöjningsfaktor_FPI*Moms</f>
         <v>568177.50000000012</v>
       </c>
@@ -1612,8 +1611,8 @@
         <v>250</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1470270270270271</v>
+        <f t="shared" si="2"/>
+        <v>1.6238993710691818</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>16</v>
@@ -1624,9 +1623,9 @@
       <c r="L8" s="7">
         <v>325</v>
       </c>
-      <c r="M8" s="12">
-        <f t="shared" si="1"/>
-        <v>1.1232142857142857</v>
+      <c r="M8" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7999999999999989</v>
       </c>
       <c r="N8" t="s">
         <v>17</v>
@@ -1634,13 +1633,13 @@
       <c r="O8" t="s">
         <v>102</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="13">
         <v>160</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="Q8" s="13">
         <v>250</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="13">
         <v>325</v>
       </c>
       <c r="S8" s="8">
@@ -1648,12 +1647,12 @@
         <v>1</v>
       </c>
       <c r="T8" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1156250000000001</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="U8" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1203125</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>15</v>
@@ -1667,13 +1666,13 @@
       <c r="Y8" s="7">
         <v>180</v>
       </c>
-      <c r="Z8" s="12">
-        <f t="shared" si="3"/>
-        <v>1.1120000000000001</v>
-      </c>
-      <c r="AA8" s="12">
-        <f t="shared" si="4"/>
-        <v>1.1180000000000001</v>
+      <c r="Z8" s="10">
+        <f t="shared" si="6"/>
+        <v>1.0711111111111111</v>
+      </c>
+      <c r="AA8" s="10">
+        <f t="shared" si="7"/>
+        <v>1.0716417910447762</v>
       </c>
       <c r="AB8" t="s">
         <v>57</v>
@@ -1693,20 +1692,20 @@
       <c r="AG8">
         <v>240</v>
       </c>
-      <c r="AH8" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH8" s="15">
+        <f t="shared" si="1"/>
         <v>2582.6250000000005</v>
       </c>
-      <c r="AI8" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI8" s="15">
+        <f t="shared" si="1"/>
         <v>2840.8874999999998</v>
       </c>
-      <c r="AJ8" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ8" s="15">
+        <f t="shared" si="1"/>
         <v>3271.3250000000007</v>
       </c>
-      <c r="AK8" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK8" s="15">
+        <f t="shared" si="1"/>
         <v>4132.2000000000007</v>
       </c>
     </row>
@@ -1727,8 +1726,8 @@
         <v>250</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="6"/>
-        <v>1.117837837837838</v>
+        <f t="shared" si="2"/>
+        <v>1.080503144654088</v>
       </c>
       <c r="J9" t="s">
         <v>17</v>
@@ -1740,8 +1739,8 @@
         <v>220</v>
       </c>
       <c r="M9" s="10">
-        <f t="shared" si="1"/>
-        <v>1.1157142857142859</v>
+        <f t="shared" si="3"/>
+        <v>1.3459459459459455</v>
       </c>
       <c r="N9" t="s">
         <v>18</v>
@@ -1763,12 +1762,12 @@
         <v>1.21875</v>
       </c>
       <c r="T9" s="10">
-        <f t="shared" si="2"/>
-        <v>1.118125</v>
+        <f t="shared" si="4"/>
+        <v>1.1015873015873017</v>
       </c>
       <c r="U9" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1243750000000001</v>
+        <f t="shared" si="5"/>
+        <v>1.1040000000000001</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>16</v>
@@ -1782,13 +1781,13 @@
       <c r="Y9" s="7">
         <v>485</v>
       </c>
-      <c r="Z9" s="12">
-        <f t="shared" si="3"/>
-        <v>1.1325000000000001</v>
-      </c>
-      <c r="AA9" s="12">
-        <f t="shared" si="4"/>
-        <v>1.1485000000000001</v>
+      <c r="Z9" s="10">
+        <f t="shared" si="6"/>
+        <v>1.8000000000000012</v>
+      </c>
+      <c r="AA9" s="10">
+        <f t="shared" si="7"/>
+        <v>1.8000000000000009</v>
       </c>
       <c r="AB9" s="7" t="s">
         <v>15</v>
@@ -1808,20 +1807,20 @@
       <c r="AG9" s="7">
         <v>280</v>
       </c>
-      <c r="AH9" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH9" s="15">
+        <f t="shared" si="1"/>
         <v>3271.3250000000007</v>
       </c>
-      <c r="AI9" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI9" s="15">
+        <f t="shared" si="1"/>
         <v>3443.5</v>
       </c>
-      <c r="AJ9" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ9" s="15">
+        <f t="shared" si="1"/>
         <v>3701.7625000000003</v>
       </c>
-      <c r="AK9" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK9" s="15">
+        <f t="shared" si="1"/>
         <v>4820.9000000000005</v>
       </c>
     </row>
@@ -1842,8 +1841,8 @@
         <v>250</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1235135135135137</v>
+        <f t="shared" si="2"/>
+        <v>1.1861635220125786</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>19</v>
@@ -1854,9 +1853,9 @@
       <c r="L10" s="7">
         <v>185</v>
       </c>
-      <c r="M10" s="12">
-        <f t="shared" si="1"/>
-        <v>1.1132142857142857</v>
+      <c r="M10" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1945945945945942</v>
       </c>
       <c r="N10" t="s">
         <v>44</v>
@@ -1878,12 +1877,12 @@
         <v>1.5</v>
       </c>
       <c r="T10" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1225000000000001</v>
+        <f t="shared" si="4"/>
+        <v>1.2793650793650795</v>
       </c>
       <c r="U10" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1300000000000001</v>
+        <f t="shared" si="5"/>
+        <v>1.248</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>47</v>
@@ -1897,13 +1896,13 @@
       <c r="Y10" s="7">
         <v>360</v>
       </c>
-      <c r="Z10" s="12">
-        <f t="shared" si="3"/>
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="AA10" s="12">
-        <f t="shared" si="4"/>
-        <v>1.1360000000000001</v>
+      <c r="Z10" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4977777777777783</v>
+      </c>
+      <c r="AA10" s="10">
+        <f t="shared" si="7"/>
+        <v>1.5014925373134336</v>
       </c>
       <c r="AB10" s="7" t="s">
         <v>16</v>
@@ -1923,20 +1922,20 @@
       <c r="AG10" s="7">
         <v>260</v>
       </c>
-      <c r="AH10" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH10" s="15">
+        <f t="shared" si="1"/>
         <v>2840.8874999999998</v>
       </c>
-      <c r="AI10" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI10" s="15">
+        <f t="shared" si="1"/>
         <v>3013.0625000000005</v>
       </c>
-      <c r="AJ10" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ10" s="15">
+        <f t="shared" si="1"/>
         <v>3443.5</v>
       </c>
-      <c r="AK10" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK10" s="15">
+        <f t="shared" si="1"/>
         <v>4476.55</v>
       </c>
     </row>
@@ -1957,8 +1956,8 @@
         <v>250</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1135135135135137</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>48</v>
@@ -1972,13 +1971,13 @@
       <c r="Y11" s="7">
         <v>420</v>
       </c>
-      <c r="Z11" s="12">
-        <f t="shared" si="3"/>
-        <v>1.1280000000000001</v>
-      </c>
-      <c r="AA11" s="12">
-        <f t="shared" si="4"/>
-        <v>1.1420000000000001</v>
+      <c r="Z11" s="10">
+        <f t="shared" si="6"/>
+        <v>1.640000000000001</v>
+      </c>
+      <c r="AA11" s="10">
+        <f t="shared" si="7"/>
+        <v>1.6447761194029857</v>
       </c>
       <c r="AB11" s="7" t="s">
         <v>47</v>
@@ -1998,20 +1997,20 @@
       <c r="AG11" s="7">
         <v>270</v>
       </c>
-      <c r="AH11" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH11" s="15">
+        <f t="shared" si="1"/>
         <v>3013.0625000000005</v>
       </c>
-      <c r="AI11" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI11" s="15">
+        <f t="shared" si="1"/>
         <v>3271.3250000000007</v>
       </c>
-      <c r="AJ11" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ11" s="15">
+        <f t="shared" si="1"/>
         <v>3615.6750000000002</v>
       </c>
-      <c r="AK11" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK11" s="15">
+        <f t="shared" si="1"/>
         <v>4648.7250000000004</v>
       </c>
     </row>
@@ -2032,8 +2031,8 @@
         <v>250</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1135135135135137</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="V12" t="s">
         <v>17</v>
@@ -2048,12 +2047,12 @@
         <v>225</v>
       </c>
       <c r="Z12" s="10">
-        <f t="shared" si="3"/>
-        <v>1.115</v>
+        <f t="shared" si="6"/>
+        <v>1.177777777777778</v>
       </c>
       <c r="AA12" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1225000000000001</v>
+        <f t="shared" si="7"/>
+        <v>1.1791044776119404</v>
       </c>
       <c r="AB12" t="s">
         <v>17</v>
@@ -2073,20 +2072,20 @@
       <c r="AG12">
         <v>315</v>
       </c>
-      <c r="AH12" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH12" s="15">
+        <f t="shared" si="1"/>
         <v>3701.7625000000003</v>
       </c>
-      <c r="AI12" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI12" s="15">
+        <f t="shared" si="1"/>
         <v>4046.1125000000002</v>
       </c>
-      <c r="AJ12" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ12" s="15">
+        <f t="shared" si="1"/>
         <v>4390.4625000000005</v>
       </c>
-      <c r="AK12" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK12" s="15">
+        <f t="shared" si="1"/>
         <v>5423.5125000000007</v>
       </c>
     </row>
@@ -2107,9 +2106,10 @@
         <v>250</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1145945945945948</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>1.020125786163522</v>
+      </c>
+      <c r="K13" s="13"/>
       <c r="V13" t="s">
         <v>18</v>
       </c>
@@ -2123,12 +2123,12 @@
         <v>380</v>
       </c>
       <c r="Z13" s="10">
-        <f t="shared" si="3"/>
-        <v>1.1240000000000001</v>
+        <f t="shared" si="6"/>
+        <v>1.4977777777777783</v>
       </c>
       <c r="AA13" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1380000000000001</v>
+        <f t="shared" si="7"/>
+        <v>1.5492537313432844</v>
       </c>
       <c r="AB13" t="s">
         <v>18</v>
@@ -2148,20 +2148,20 @@
       <c r="AG13">
         <v>300</v>
       </c>
-      <c r="AH13" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH13" s="15">
+        <f t="shared" si="1"/>
         <v>3443.5</v>
       </c>
-      <c r="AI13" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI13" s="15">
+        <f t="shared" si="1"/>
         <v>3701.7625000000003</v>
       </c>
-      <c r="AJ13" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ13" s="15">
+        <f t="shared" si="1"/>
         <v>4132.2000000000007</v>
       </c>
-      <c r="AK13" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK13" s="15">
+        <f t="shared" si="1"/>
         <v>5165.2500000000009</v>
       </c>
     </row>
@@ -2182,8 +2182,8 @@
         <v>250</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1162162162162164</v>
+        <f t="shared" si="2"/>
+        <v>1.050314465408805</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>19</v>
@@ -2195,11 +2195,11 @@
         <v>220</v>
       </c>
       <c r="Y14" s="7"/>
-      <c r="Z14" s="12">
-        <f>1.1+(X14/jmfpris_yttertak)/100</f>
-        <v>1.1220000000000001</v>
-      </c>
-      <c r="AA14" s="12"/>
+      <c r="Z14" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4266666666666672</v>
+      </c>
+      <c r="AA14" s="10"/>
       <c r="AB14" t="s">
         <v>44</v>
       </c>
@@ -2218,20 +2218,20 @@
       <c r="AG14">
         <v>315</v>
       </c>
-      <c r="AH14" s="16">
-        <f t="shared" si="5"/>
+      <c r="AH14" s="15">
+        <f t="shared" si="1"/>
         <v>3615.6750000000002</v>
       </c>
-      <c r="AI14" s="16">
-        <f t="shared" si="5"/>
+      <c r="AI14" s="15">
+        <f t="shared" si="1"/>
         <v>4046.1125000000002</v>
       </c>
-      <c r="AJ14" s="16">
-        <f t="shared" si="5"/>
+      <c r="AJ14" s="15">
+        <f t="shared" si="1"/>
         <v>4390.4625000000005</v>
       </c>
-      <c r="AK14" s="16">
-        <f t="shared" si="5"/>
+      <c r="AK14" s="15">
+        <f t="shared" si="1"/>
         <v>5423.5125000000007</v>
       </c>
     </row>
@@ -2252,9 +2252,10 @@
         <v>250</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1172972972972974</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>1.070440251572327</v>
+      </c>
+      <c r="K15" s="7"/>
       <c r="V15" t="s">
         <v>20</v>
       </c>
@@ -2268,12 +2269,12 @@
         <v>260</v>
       </c>
       <c r="Z15" s="10">
-        <f>1.1+(X15/jmfpris_yttertak)/100</f>
-        <v>1.1175000000000002</v>
+        <f t="shared" si="6"/>
+        <v>1.2666666666666671</v>
       </c>
       <c r="AA15" s="10">
-        <f>1.1+(Y15/jmfpris_yttertak)/100</f>
-        <v>1.1260000000000001</v>
+        <f t="shared" si="7"/>
+        <v>1.2626865671641794</v>
       </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.25">
@@ -2293,11 +2294,13 @@
         <v>250</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="6"/>
-        <v>1.117837837837838</v>
-      </c>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.080503144654088</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D17" s="7" t="s">
         <v>28</v>
       </c>
@@ -2314,11 +2317,12 @@
         <v>250</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1154054054054054</v>
-      </c>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.0352201257861635</v>
+      </c>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D18" s="7" t="s">
         <v>28</v>
       </c>
@@ -2335,11 +2339,13 @@
         <v>250</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1164864864864865</v>
-      </c>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.0553459119496855</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2356,11 +2362,12 @@
         <v>250</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1170270270270271</v>
-      </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.0654088050314465</v>
+      </c>
+      <c r="W19" s="12"/>
+    </row>
+    <row r="20" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>29</v>
       </c>
@@ -2377,11 +2384,11 @@
         <v>250</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.93459119496855347</v>
+      </c>
+    </row>
+    <row r="21" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>29</v>
       </c>
@@ -2398,11 +2405,11 @@
         <v>250</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1121621621621622</v>
-      </c>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.97484276729559749</v>
+      </c>
+    </row>
+    <row r="22" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>29</v>
       </c>
@@ -2419,11 +2426,13 @@
         <v>250</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1140540540540542</v>
-      </c>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.010062893081761</v>
+      </c>
+      <c r="W22" s="7"/>
+      <c r="Z22" s="7"/>
+    </row>
+    <row r="23" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>29</v>
       </c>
@@ -2440,11 +2449,13 @@
         <v>250</v>
       </c>
       <c r="I23" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1154054054054054</v>
-      </c>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.0352201257861635</v>
+      </c>
+      <c r="W23" s="7"/>
+      <c r="Z23" s="7"/>
+    </row>
+    <row r="24" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2461,11 +2472,13 @@
         <v>250</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1124324324324326</v>
-      </c>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.97987421383647799</v>
+      </c>
+      <c r="W24" s="7"/>
+      <c r="Z24" s="7"/>
+    </row>
+    <row r="25" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>29</v>
       </c>
@@ -2482,11 +2495,13 @@
         <v>250</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1132432432432433</v>
-      </c>
-    </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.9949685534591195</v>
+      </c>
+      <c r="W25" s="7"/>
+      <c r="Z25" s="7"/>
+    </row>
+    <row r="26" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D26" s="7" t="s">
         <v>29</v>
       </c>
@@ -2503,11 +2518,11 @@
         <v>250</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1162162162162164</v>
-      </c>
-    </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.050314465408805</v>
+      </c>
+    </row>
+    <row r="27" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D27" s="7" t="s">
         <v>29</v>
       </c>
@@ -2524,11 +2539,11 @@
         <v>250</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1183783783783785</v>
-      </c>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.090566037735849</v>
+      </c>
+    </row>
+    <row r="28" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
         <v>29</v>
       </c>
@@ -2545,11 +2560,13 @@
         <v>250</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.120754716981132</v>
+      </c>
+      <c r="W28" s="7"/>
+      <c r="Z28" s="7"/>
+    </row>
+    <row r="29" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
         <v>29</v>
       </c>
@@ -2566,11 +2583,11 @@
         <v>250</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="6"/>
-        <v>1.117837837837838</v>
-      </c>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.080503144654088</v>
+      </c>
+    </row>
+    <row r="30" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D30" s="7" t="s">
         <v>29</v>
       </c>
@@ -2587,18 +2604,60 @@
         <v>250</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="6"/>
-        <v>1.1216216216216217</v>
-      </c>
-    </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1.1509433962264151</v>
+      </c>
+    </row>
+    <row r="31" spans="4:26" x14ac:dyDescent="0.25">
       <c r="N31" s="10"/>
     </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="7"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="7"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="7"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="7"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F34:F59">
+    <sortCondition ref="F34:F59"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB19" xr:uid="{81FA3817-5029-4E85-B009-42D1A0154D3B}">
-      <formula1>$Z$18:$Z$21</formula1>
+      <formula1>$Z$18:$Z$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>